<commit_message>
Cost of debt computation
</commit_message>
<xml_diff>
--- a/Project/Work in progress/Simone's part.xlsx
+++ b/Project/Work in progress/Simone's part.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\Corporate-project-\Project\Work in progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2266" documentId="13_ncr:1_{2EE670BD-D333-445C-855D-43AC8679340C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DE286CCA-F883-4488-AA2E-B8D6909396D2}"/>
+  <xr:revisionPtr revIDLastSave="2286" documentId="13_ncr:1_{2EE670BD-D333-445C-855D-43AC8679340C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CDCBBD1-DCC9-4D87-9B8C-4F6A633C9B82}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IS" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="567">
   <si>
     <t>Ricavi</t>
   </si>
@@ -1729,6 +1729,30 @@
   </si>
   <si>
     <t>Market cap (at 31/12/19)</t>
+  </si>
+  <si>
+    <t>Outstanding bonds</t>
+  </si>
+  <si>
+    <t>Bond2022</t>
+  </si>
+  <si>
+    <t>Bond2025</t>
+  </si>
+  <si>
+    <t>bond2027</t>
+  </si>
+  <si>
+    <t>bond2029</t>
+  </si>
+  <si>
+    <t>Yield to maturity</t>
+  </si>
+  <si>
+    <t>Residual Coup</t>
+  </si>
+  <si>
+    <t>Average Kd</t>
   </si>
 </sst>
 </file>
@@ -2757,7 +2781,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="272">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3064,6 +3088,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Migliaia" xfId="2" builtinId="3"/>
@@ -11954,8 +11979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453EC5EB-3EA3-41FC-BD61-B127DEE946BB}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11965,11 +11990,13 @@
     <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" customWidth="1"/>
     <col min="7" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="12" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
     <col min="13" max="13" width="12.109375" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="12" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="0.88671875" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="10.5546875" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="11.6640625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="13.44140625" hidden="1" customWidth="1"/>
@@ -12600,8 +12627,8 @@
       <c r="G39" s="96"/>
       <c r="H39" s="97"/>
     </row>
-    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="150" t="s">
         <v>541</v>
       </c>
@@ -12610,16 +12637,38 @@
       <c r="D66" s="93"/>
       <c r="E66" s="93"/>
       <c r="F66" s="94"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I66" s="98"/>
+      <c r="J66" s="98" t="s">
+        <v>564</v>
+      </c>
+      <c r="K66" s="98" t="s">
+        <v>565</v>
+      </c>
+      <c r="L66" s="98" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="151"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="F67" s="95"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I67" s="98" t="s">
+        <v>560</v>
+      </c>
+      <c r="J67" s="98">
+        <v>3.6880000000000003E-2</v>
+      </c>
+      <c r="K67" s="98">
+        <v>2</v>
+      </c>
+      <c r="L67" s="98">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="151" t="s">
         <v>553</v>
       </c>
@@ -12634,8 +12683,20 @@
       <c r="F68" s="257">
         <v>-7.2081146095294803E-4</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I68" s="98" t="s">
+        <v>561</v>
+      </c>
+      <c r="J68" s="98">
+        <v>1.8360000000000001E-2</v>
+      </c>
+      <c r="K68" s="98">
+        <v>5</v>
+      </c>
+      <c r="L68" s="98">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="151" t="s">
         <v>554</v>
       </c>
@@ -12650,8 +12711,20 @@
       <c r="F69" s="258">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I69" s="98" t="s">
+        <v>562</v>
+      </c>
+      <c r="J69" s="98">
+        <v>1.7680000000000001E-2</v>
+      </c>
+      <c r="K69" s="98">
+        <v>8</v>
+      </c>
+      <c r="L69" s="98">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="263" t="s">
         <v>543</v>
       </c>
@@ -12668,8 +12741,20 @@
         <f t="shared" ref="F70" si="6">SUM(F68:F69)</f>
         <v>1.4279188539047052E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I70" s="98" t="s">
+        <v>563</v>
+      </c>
+      <c r="J70" s="98">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="K70" s="98">
+        <v>10</v>
+      </c>
+      <c r="L70" s="98">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="151"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -12677,7 +12762,7 @@
       <c r="E71" s="6"/>
       <c r="F71" s="95"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="151" t="s">
         <v>542</v>
       </c>
@@ -12692,8 +12777,15 @@
       <c r="F72" s="257">
         <v>-7.2081146095294803E-4</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I72" s="200" t="s">
+        <v>566</v>
+      </c>
+      <c r="J72" s="272">
+        <f xml:space="preserve"> (PRODUCT(J67:L67) + PRODUCT(J68:L68) + PRODUCT(J69:L69) + PRODUCT(J70:L70)) / (PRODUCT(K67:L67) + PRODUCT(K68:L68) + PRODUCT(K69:L69) + PRODUCT(K70:L70))</f>
+        <v>1.8253033707865168E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="151" t="s">
         <v>555</v>
       </c>
@@ -12709,7 +12801,7 @@
         <v>2.99661426831043E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="151" t="s">
         <v>556</v>
       </c>
@@ -12725,7 +12817,7 @@
         <v>4.02051047177864</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="151" t="s">
         <v>557</v>
       </c>
@@ -12740,7 +12832,7 @@
       <c r="E75" s="6"/>
       <c r="F75" s="95"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="151" t="s">
         <v>544</v>
       </c>
@@ -12754,7 +12846,7 @@
       <c r="E76" s="250"/>
       <c r="F76" s="95"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="151" t="s">
         <v>545</v>
       </c>
@@ -12769,7 +12861,7 @@
       <c r="E77" s="6"/>
       <c r="F77" s="95"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="151"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -12777,7 +12869,7 @@
       <c r="E78" s="6"/>
       <c r="F78" s="95"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="151" t="s">
         <v>546</v>
       </c>
@@ -12791,7 +12883,7 @@
       <c r="E79" s="6"/>
       <c r="F79" s="95"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="151"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -12910,7 +13002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71461D4C-151F-470B-8443-1903C71474D2}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>